<commit_message>
Updated robot to get transaction details from Orchestrator Queue
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\patricio.c.calacasan\Documents\UiPath\RemoteAutomationFramework_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A45D17CA-6E00-4F61-B9ED-8D15CA816A7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF86CB-D743-47F7-83AB-DA5A2F5EBE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>Name</t>
   </si>
@@ -116,37 +116,19 @@
     <t>OrchestratorAssetFolder</t>
   </si>
   <si>
-    <t>TestExecutionQueue</t>
-  </si>
-  <si>
     <t>OrchestratorQueueName</t>
   </si>
   <si>
     <t>OrchestratorFolderPath</t>
   </si>
   <si>
-    <t>(IFL) International Fuel and Lubricant</t>
+    <t>Generic Asset</t>
   </si>
   <si>
-    <t>Folder path for the Queue Name</t>
+    <t>ExecutionQueue</t>
   </si>
   <si>
-    <t>SharedRepository</t>
-  </si>
-  <si>
-    <t>C:\temp</t>
-  </si>
-  <si>
-    <t>DelayLong</t>
-  </si>
-  <si>
-    <t>DelayShort</t>
-  </si>
-  <si>
-    <t>00:00:10</t>
-  </si>
-  <si>
-    <t>00:00:01</t>
+    <t>FolderLocation_ExecutionFile</t>
   </si>
 </sst>
 </file>
@@ -523,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1001"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -573,10 +555,10 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
@@ -584,53 +566,29 @@
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
         <v>32</v>
-      </c>
-      <c r="B3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>36</v>
-      </c>
+      <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="14.25" customHeight="1">
+    <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1">
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:26" ht="30">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1621,9 +1579,6 @@
     <row r="996" ht="14.25" customHeight="1"/>
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-    <row r="1001" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2744,10 +2699,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2794,7 +2749,17 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+    </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:26" ht="14.25" customHeight="1"/>
@@ -3792,7 +3757,6 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
     <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated variable Reference to QueueReference
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AF86CB-D743-47F7-83AB-DA5A2F5EBE57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D23DB6-26D9-4100-B22A-8A76DB852448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>LogMessage_GetTransactionData</t>
   </si>
   <si>
-    <t xml:space="preserve">Processing Transaction Number: </t>
-  </si>
-  <si>
     <t>LogMessage_GetTransactionDataError</t>
   </si>
   <si>
@@ -67,9 +64,6 @@
   </si>
   <si>
     <t>LogMessage_Success</t>
-  </si>
-  <si>
-    <t>Transaction Successful.</t>
   </si>
   <si>
     <t>LogMessage_BusinessRuleException</t>
@@ -129,6 +123,12 @@
   </si>
   <si>
     <t>FolderLocation_ExecutionFile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">********Processing Transaction Number: </t>
+  </si>
+  <si>
+    <t>********Transaction Successful.</t>
   </si>
 </sst>
 </file>
@@ -507,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -555,21 +555,21 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -577,13 +577,13 @@
     </row>
     <row r="5" spans="1:26" ht="30">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1590,7 +1590,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
@@ -1642,7 +1644,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1663,54 +1665,54 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2721,7 +2723,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
@@ -2751,13 +2753,13 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
May 21, 2022 01:41AM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98DCA41-7287-43D2-9CF3-53BCC6DF199A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2413C1E4-034C-48FF-B924-A0E58C951A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>******************Business rule exception******************</t>
+  </si>
+  <si>
+    <t>FolderLocation_UserInterface</t>
   </si>
 </sst>
 </file>
@@ -1599,8 +1602,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z987"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2712,8 +2715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2804,7 +2807,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="9" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
June 21, 2022 09:44AM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2413C1E4-034C-48FF-B924-A0E58C951A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0416757F-6692-48D3-9C7B-E387E7772F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>FolderLocation_UserInterface</t>
+  </si>
+  <si>
+    <t>Delay_Medium</t>
+  </si>
+  <si>
+    <t>NumberOfRetries</t>
+  </si>
+  <si>
+    <t>RetryInterval</t>
   </si>
 </sst>
 </file>
@@ -2716,7 +2725,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2818,9 +2827,39 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
July 04, 2022 01:40PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0416757F-6692-48D3-9C7B-E387E7772F9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656BF0A4-2ED7-4658-9DC1-43EF60A3CBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>RetryInterval</t>
+  </si>
+  <si>
+    <t>AssetName_Credential_ORBIS_KH</t>
   </si>
 </sst>
 </file>
@@ -2725,13 +2728,13 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" customWidth="1"/>
+    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
@@ -2860,7 +2863,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
July 08, 2022 04:17PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{656BF0A4-2ED7-4658-9DC1-43EF60A3CBDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135D2FBD-B307-4254-BC87-841AA8543A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
   <si>
     <t>Name</t>
   </si>
@@ -153,6 +153,12 @@
   </si>
   <si>
     <t>AssetName_Credential_ORBIS_KH</t>
+  </si>
+  <si>
+    <t>Delay_DIspenseFuel</t>
+  </si>
+  <si>
+    <t>Amount_ManualDelivery_Pump3_Diesel_ManualFuelSale</t>
   </si>
 </sst>
 </file>
@@ -2728,13 +2734,12 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="60.28515625" customWidth="1"/>
     <col min="4" max="26" width="65.42578125" customWidth="1"/>
   </cols>
@@ -2874,8 +2879,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
September 09, 2022 11:32PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135D2FBD-B307-4254-BC87-841AA8543A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A064E0-BB19-40A3-B9E7-49FD518AFF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
   <si>
     <t>Name</t>
   </si>
@@ -159,6 +159,45 @@
   </si>
   <si>
     <t>Amount_ManualDelivery_Pump3_Diesel_ManualFuelSale</t>
+  </si>
+  <si>
+    <t>Amount_ManualDelivery_Pump4_SilverTechron_ManualFuelSale</t>
+  </si>
+  <si>
+    <t>Amount_ManualDelivery_Pump3_SilverTechron_ManualFuelSale</t>
+  </si>
+  <si>
+    <t>ReasonForRefund_CancelSale</t>
+  </si>
+  <si>
+    <t>Registration_DriveOff</t>
+  </si>
+  <si>
+    <t>Make_DriveOff</t>
+  </si>
+  <si>
+    <t>Model_DriveOff</t>
+  </si>
+  <si>
+    <t>Type_DriveOff</t>
+  </si>
+  <si>
+    <t>Colour_DriveOff</t>
+  </si>
+  <si>
+    <t>DriverDescription_DriveOff</t>
+  </si>
+  <si>
+    <t>Comment_DriveOff</t>
+  </si>
+  <si>
+    <t>ItemNumber_Drystock</t>
+  </si>
+  <si>
+    <t>Amount_ManualDelivery_Pump3_GoldTechron_ManualFuelSale</t>
+  </si>
+  <si>
+    <t>Selector_CVScreenScope</t>
   </si>
 </sst>
 </file>
@@ -176,6 +215,7 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="6"/>
@@ -541,12 +581,12 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -605,7 +645,7 @@
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>17</v>
       </c>
@@ -1624,12 +1664,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1666,7 +1706,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -2733,15 +2773,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="53.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="2" width="55.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -2901,26 +2941,156 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
September 13, 2022 08:47PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A064E0-BB19-40A3-B9E7-49FD518AFF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0F6E10-D799-4A9F-9E06-515AF60E30F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -198,6 +198,9 @@
   </si>
   <si>
     <t>Selector_CVScreenScope</t>
+  </si>
+  <si>
+    <t>Delay_Long</t>
   </si>
 </sst>
 </file>
@@ -2773,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3084,7 +3087,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="26" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
September 19, 2022 02:22PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D0F6E10-D799-4A9F-9E06-515AF60E30F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52EF009-43D3-4258-81BB-8AB71F5B2C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Delay_Long</t>
+  </si>
+  <si>
+    <t>NewQuantity</t>
   </si>
 </sst>
 </file>
@@ -2777,7 +2780,7 @@
   <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="C26" sqref="A26:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3098,7 +3101,17 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="27" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="30" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
September 20, 2022 05:28PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F52EF009-43D3-4258-81BB-8AB71F5B2C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF1AFA0-ABA7-4D65-A1C8-406F57AF7219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -204,6 +204,24 @@
   </si>
   <si>
     <t>NewQuantity</t>
+  </si>
+  <si>
+    <t>CurrencyCode_New</t>
+  </si>
+  <si>
+    <t>ExchangeRate_New</t>
+  </si>
+  <si>
+    <t>SellingRate_New</t>
+  </si>
+  <si>
+    <t>BuyingRate_New</t>
+  </si>
+  <si>
+    <t>UseDrawer_New</t>
+  </si>
+  <si>
+    <t>UseDrawer_EditCurrency</t>
   </si>
 </sst>
 </file>
@@ -2779,8 +2797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C26" sqref="A26:C27"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3112,27 +3130,87 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="29" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="30" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="31" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="32" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="28" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="40" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="47" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="49" ht="14.25" customHeight="1"/>
     <row r="50" ht="14.25" customHeight="1"/>
     <row r="51" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
September 21, 2022 051:14PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF1AFA0-ABA7-4D65-A1C8-406F57AF7219}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B4289A-6289-4E10-84B7-75F102914087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -222,6 +222,12 @@
   </si>
   <si>
     <t>UseDrawer_EditCurrency</t>
+  </si>
+  <si>
+    <t>Amount_PayIn</t>
+  </si>
+  <si>
+    <t>Amount_PayOut</t>
   </si>
 </sst>
 </file>
@@ -2797,8 +2803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3196,8 +3202,28 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="14.25" customHeight="1"/>
-    <row r="35" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="34" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
October 10, 2022 08:37PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\srcCode\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54B4289A-6289-4E10-84B7-75F102914087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B71F83A-AF57-4DF5-BB59-CE59362C9E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -113,9 +113,6 @@
     <t>OrchestratorFolderPath</t>
   </si>
   <si>
-    <t>Generic Asset</t>
-  </si>
-  <si>
     <t>ExecutionQueue</t>
   </si>
   <si>
@@ -228,6 +225,12 @@
   </si>
   <si>
     <t>Amount_PayOut</t>
+  </si>
+  <si>
+    <t>Downstream/International Products/IFL Automation</t>
+  </si>
+  <si>
+    <t>Amount_SafeDropLimit</t>
   </si>
 </sst>
 </file>
@@ -608,7 +611,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -658,7 +661,7 @@
         <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>19</v>
@@ -669,7 +672,7 @@
         <v>28</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
@@ -1765,7 +1768,7 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>25</v>
@@ -1787,7 +1790,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1798,7 +1801,7 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" t="s">
         <v>23</v>
@@ -2803,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -2852,379 +2855,386 @@
     </row>
     <row r="2" spans="1:26" ht="14.25" customHeight="1">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="14.25" customHeight="1">
       <c r="A3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="14.25" customHeight="1">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>29</v>
+        <v>47</v>
+      </c>
+      <c r="C16" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>29</v>
+        <v>49</v>
+      </c>
+      <c r="C18" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>29</v>
+        <v>50</v>
+      </c>
+      <c r="C19" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="14.25" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>29</v>
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>29</v>
+        <v>53</v>
+      </c>
+      <c r="C22" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>29</v>
+        <v>54</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>29</v>
+        <v>55</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>29</v>
+        <v>56</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
+      </c>
+      <c r="C26" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>29</v>
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>29</v>
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>29</v>
+        <v>62</v>
+      </c>
+      <c r="C31" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>29</v>
+        <v>63</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="14.25" customHeight="1">
       <c r="A33" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>29</v>
+        <v>64</v>
+      </c>
+      <c r="C33" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="14.25" customHeight="1">
       <c r="A34" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>29</v>
+        <v>65</v>
+      </c>
+      <c r="C34" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="14.25" customHeight="1">
       <c r="A35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
         <v>67</v>
       </c>
-      <c r="B35" s="2" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="B36" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="14.25" customHeight="1"/>
+    </row>
     <row r="37" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="39" spans="1:3" ht="14.25" customHeight="1"/>

</xml_diff>

<commit_message>
October 10, 2022 10:12PM
</commit_message>
<xml_diff>
--- a/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
+++ b/TestAutomation_GenericAsset/TestAutomation_GenericAsset_Performer/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UiPath_TestAutomation_GenericAsset\TestAutomation_GenericAsset\TestAutomation_GenericAsset_Performer\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B71F83A-AF57-4DF5-BB59-CE59362C9E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34FBFCE2-21D3-4D06-926E-387C3E2218FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="69">
   <si>
     <t>Name</t>
   </si>
@@ -2806,8 +2806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B24" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -3228,6 +3228,9 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A36" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="B36" s="2" t="s">
         <v>68</v>
       </c>

</xml_diff>